<commit_message>
Results for `ray` were the same as the ones for `graphic`, fix this
</commit_message>
<xml_diff>
--- a/doors/results/doors_desktop.xlsx
+++ b/doors/results/doors_desktop.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="9480" tabRatio="991" activeTab="2"/>
+    <workbookView windowWidth="23025" windowHeight="9990" tabRatio="991" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="doors_desktop" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="621">
   <si>
     <t>name</t>
   </si>
@@ -1874,6 +1874,12 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Quartile 25%</t>
+  </si>
+  <si>
+    <t>Quartile 75%</t>
   </si>
 </sst>
 </file>
@@ -1883,9 +1889,9 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1894,34 +1900,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1933,24 +1915,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1973,14 +1956,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1995,7 +1978,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2008,40 +2021,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2054,7 +2060,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2066,7 +2102,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2078,19 +2174,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2102,7 +2198,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2114,127 +2234,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2253,6 +2259,65 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2276,7 +2341,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2295,200 +2360,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -15522,12 +15528,13 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E7" sqref="E7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="3" width="10.5714285714286"/>
+    <col min="5" max="5" width="12.5714285714286" customWidth="1"/>
     <col min="6" max="8" width="8.71428571428571" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16741,12 +16748,16 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="3" width="9.71428571428571"/>
+    <col min="5" max="5" width="12.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="9.57142857142857"/>
+    <col min="7" max="7" width="10.5714285714286"/>
+    <col min="8" max="8" width="9.57142857142857"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -16899,7 +16910,7 @@
         <v>8846.64</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>4892.54</v>
       </c>
@@ -16909,8 +16920,23 @@
       <c r="C7" s="2">
         <v>7442.66</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="E7" t="s">
+        <v>619</v>
+      </c>
+      <c r="F7">
+        <f>QUARTILE(Table2[50%],1)</f>
+        <v>4923.29</v>
+      </c>
+      <c r="G7">
+        <f>QUARTILE(Table2[70%],1)</f>
+        <v>5512.3725</v>
+      </c>
+      <c r="H7">
+        <f>QUARTILE(Table2[90%],1)</f>
+        <v>7813.495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>4860.93</v>
       </c>
@@ -16919,6 +16945,21 @@
       </c>
       <c r="C8" s="2">
         <v>7697.47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>620</v>
+      </c>
+      <c r="F8">
+        <f>QUARTILE(Table2[50%],3)</f>
+        <v>4967.585</v>
+      </c>
+      <c r="G8">
+        <f>QUARTILE(Table2[70%],3)</f>
+        <v>5853.8325</v>
+      </c>
+      <c r="H8">
+        <f>QUARTILE(Table2[90%],3)</f>
+        <v>8210.55</v>
       </c>
     </row>
     <row r="9" spans="1:3">

</xml_diff>